<commit_message>
Docs: Se agregan trabajos
</commit_message>
<xml_diff>
--- a/Primer_Trimestres/Nomalizacion/correccion/Normalización .xlsx
+++ b/Primer_Trimestres/Nomalizacion/correccion/Normalización .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d01d89a1400d5043/Documentos/FARMIFARMACY/Docs excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{5D5CD52F-53E4-4F0F-B9B6-38621EE8DA4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AF730BA1-46E8-49F3-B006-2027590EA4E5}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{5D5CD52F-53E4-4F0F-B9B6-38621EE8DA4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{43EF1CC0-5624-4CB7-95D0-D640E49D8568}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="4" activeTab="7" xr2:uid="{EB7CC955-6B47-4A67-9DA5-CC93A65E4CC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="3" activeTab="7" xr2:uid="{EB7CC955-6B47-4A67-9DA5-CC93A65E4CC7}"/>
   </bookViews>
   <sheets>
     <sheet name="cliente" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="276">
   <si>
     <t>identificacion</t>
   </si>
@@ -836,6 +836,30 @@
   </si>
   <si>
     <t>VENDEDOR-ROL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imagen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">aceite de bacalao.jpg </t>
+  </si>
+  <si>
+    <t>jarabe abrilar.jpg</t>
+  </si>
+  <si>
+    <t>caja de acetaminofén.jpg</t>
+  </si>
+  <si>
+    <t>jarabe acetaminofén.jpg</t>
+  </si>
+  <si>
+    <t>acetaminofén en gotas.jpg</t>
+  </si>
+  <si>
+    <t>acetato de aluminio caja.jpg</t>
+  </si>
+  <si>
+    <t>acetilcisteína en polvo.jpg</t>
   </si>
 </sst>
 </file>
@@ -1181,6 +1205,7 @@
     <xf numFmtId="164" fontId="0" fillId="18" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1190,7 +1215,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1205,14 +1233,10 @@
     <xf numFmtId="0" fontId="4" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2470,7 +2494,7 @@
       </c>
       <c r="D2" s="15">
         <f ca="1">NOW()</f>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E2" s="15">
         <v>44673.458333333336</v>
@@ -2488,7 +2512,7 @@
       </c>
       <c r="D3" s="15">
         <f t="shared" ref="D3:D20" ca="1" si="0">NOW()</f>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E3" s="15">
         <v>44674.458333333336</v>
@@ -2506,7 +2530,7 @@
       </c>
       <c r="D4" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E4" s="15">
         <v>44675.458333333336</v>
@@ -2524,7 +2548,7 @@
       </c>
       <c r="D5" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E5" s="15">
         <v>44676.458333333336</v>
@@ -2542,7 +2566,7 @@
       </c>
       <c r="D6" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E6" s="15">
         <v>44677.458333333336</v>
@@ -2560,7 +2584,7 @@
       </c>
       <c r="D7" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E7" s="15">
         <v>44678.458333333336</v>
@@ -2578,7 +2602,7 @@
       </c>
       <c r="D8" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E8" s="15">
         <v>44679.458333333336</v>
@@ -2596,7 +2620,7 @@
       </c>
       <c r="D9" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E9" s="15">
         <v>44680.458333333336</v>
@@ -2614,7 +2638,7 @@
       </c>
       <c r="D10" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E10" s="15">
         <v>44681.458333333336</v>
@@ -2632,7 +2656,7 @@
       </c>
       <c r="D11" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E11" s="15">
         <v>44682.458333333336</v>
@@ -2650,7 +2674,7 @@
       </c>
       <c r="D12" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E12" s="15">
         <v>44683.458333333336</v>
@@ -2668,7 +2692,7 @@
       </c>
       <c r="D13" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E13" s="15">
         <v>44684.458333333336</v>
@@ -2686,7 +2710,7 @@
       </c>
       <c r="D14" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E14" s="15">
         <v>44685.458333333336</v>
@@ -2704,7 +2728,7 @@
       </c>
       <c r="D15" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E15" s="15">
         <v>44686.458333333336</v>
@@ -2722,7 +2746,7 @@
       </c>
       <c r="D16" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E16" s="15">
         <v>44687.458333333336</v>
@@ -2740,7 +2764,7 @@
       </c>
       <c r="D17" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E17" s="15">
         <v>44688.458333333336</v>
@@ -2758,7 +2782,7 @@
       </c>
       <c r="D18" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E18" s="15">
         <v>44689.458333333336</v>
@@ -2776,7 +2800,7 @@
       </c>
       <c r="D19" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E19" s="15">
         <v>44690.458333333336</v>
@@ -2794,7 +2818,7 @@
       </c>
       <c r="D20" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
       <c r="E20" s="15">
         <v>44691.458333333336</v>
@@ -2993,63 +3017,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="51">
+      <c r="B1" s="53"/>
+      <c r="C1" s="52">
         <v>1192831945</v>
       </c>
-      <c r="D1" s="51"/>
+      <c r="D1" s="52"/>
       <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="5">
         <f ca="1">NOW()</f>
-        <v>44316.597251157407</v>
+        <v>44319.803879050924</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="53" t="s">
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="53"/>
+      <c r="F2" s="54"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="51">
+      <c r="B4" s="52">
         <v>3172727783</v>
       </c>
-      <c r="C4" s="51"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="51"/>
+      <c r="F4" s="52"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -3242,39 +3266,39 @@
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51" t="s">
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="51"/>
+      <c r="E16" s="52"/>
       <c r="F16" s="6">
         <v>389</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51" t="s">
+      <c r="A17" s="52"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="51"/>
+      <c r="E17" s="52"/>
       <c r="F17" s="6">
         <v>73.91</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51" t="s">
+      <c r="A18" s="52"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="51"/>
+      <c r="E18" s="52"/>
       <c r="F18" s="6">
         <v>462.90999999999997</v>
       </c>
@@ -3318,7 +3342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C30745-176D-41BA-8D9A-0B39EE9C6969}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
@@ -4814,8 +4838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{154A3EB2-7D84-4648-B4B7-AFD12D379634}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41:E41"/>
+    <sheetView topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5127,16 +5151,16 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="55" t="s">
         <v>242</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
@@ -5411,18 +5435,18 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="58" t="s">
         <v>239</v>
       </c>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="G25" s="58" t="s">
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="G25" s="60" t="s">
         <v>244</v>
       </c>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
     </row>
     <row r="26" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -5444,6 +5468,9 @@
       <c r="G27" s="41" t="s">
         <v>141</v>
       </c>
+      <c r="H27" s="41" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
@@ -5464,6 +5491,9 @@
       <c r="G28" s="42">
         <v>43</v>
       </c>
+      <c r="H28" s="41" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="s">
@@ -5484,6 +5514,9 @@
       <c r="G29" s="42">
         <v>76</v>
       </c>
+      <c r="H29" s="41" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="36" t="s">
@@ -5504,6 +5537,9 @@
       <c r="G30" s="42">
         <v>8</v>
       </c>
+      <c r="H30" s="41" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
@@ -5524,6 +5560,9 @@
       <c r="G31" s="42">
         <v>6</v>
       </c>
+      <c r="H31" s="41" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="36" t="s">
@@ -5544,8 +5583,11 @@
       <c r="G32" s="42">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="41" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="36" t="s">
         <v>237</v>
       </c>
@@ -5564,8 +5606,11 @@
       <c r="G33" s="42">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="41" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="36" t="s">
         <v>238</v>
       </c>
@@ -5584,20 +5629,24 @@
       <c r="G34" s="42">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="57" t="s">
+      <c r="H34" s="41" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="59" t="s">
         <v>228</v>
       </c>
-      <c r="B35" s="57"/>
-      <c r="D35" s="54" t="s">
+      <c r="B35" s="59"/>
+      <c r="D35" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="54"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="54"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="61"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="43" t="s">
         <v>230</v>
       </c>
@@ -5607,11 +5656,11 @@
       <c r="D37" s="48" t="s">
         <v>257</v>
       </c>
-      <c r="E37" s="61" t="s">
+      <c r="E37" s="51" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
         <v>178</v>
       </c>
@@ -5621,11 +5670,11 @@
       <c r="D38" s="48" t="s">
         <v>262</v>
       </c>
-      <c r="E38" s="61" t="s">
+      <c r="E38" s="51" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="43" t="s">
         <v>249</v>
       </c>
@@ -5635,11 +5684,11 @@
       <c r="D39" s="48" t="s">
         <v>263</v>
       </c>
-      <c r="E39" s="61" t="s">
+      <c r="E39" s="51" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
         <v>251</v>
       </c>
@@ -5649,29 +5698,29 @@
       <c r="D40" s="48" t="s">
         <v>264</v>
       </c>
-      <c r="E40" s="61" t="s">
+      <c r="E40" s="51" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="55" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="57" t="s">
         <v>252</v>
       </c>
-      <c r="B41" s="55"/>
-      <c r="D41" s="62" t="s">
+      <c r="B41" s="57"/>
+      <c r="D41" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="E41" s="62"/>
+      <c r="E41" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D35:G35"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="G25:I25"/>
+    <mergeCell ref="D35:H35"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -5695,8 +5744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C15CDDD0-1EC6-46EB-86DD-BB5C7073D9F7}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6001,22 +6050,22 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="62" t="s">
         <v>240</v>
       </c>
-      <c r="B12" s="60"/>
-      <c r="D12" s="60" t="s">
+      <c r="B12" s="62"/>
+      <c r="D12" s="62" t="s">
         <v>255</v>
       </c>
-      <c r="E12" s="60"/>
-      <c r="G12" s="60" t="s">
+      <c r="E12" s="62"/>
+      <c r="G12" s="62" t="s">
         <v>241</v>
       </c>
-      <c r="H12" s="60"/>
-      <c r="J12" s="60" t="s">
+      <c r="H12" s="62"/>
+      <c r="J12" s="62" t="s">
         <v>256</v>
       </c>
-      <c r="K12" s="60"/>
+      <c r="K12" s="62"/>
     </row>
     <row r="13" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G13"/>
@@ -6312,29 +6361,29 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="60" t="s">
+      <c r="A25" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="B25" s="60"/>
-      <c r="D25" s="60" t="s">
+      <c r="B25" s="62"/>
+      <c r="D25" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="E25" s="60"/>
-      <c r="G25" s="60" t="s">
+      <c r="E25" s="62"/>
+      <c r="G25" s="62" t="s">
         <v>266</v>
       </c>
-      <c r="H25" s="60"/>
-      <c r="J25" s="60" t="s">
+      <c r="H25" s="62"/>
+      <c r="J25" s="62" t="s">
         <v>267</v>
       </c>
-      <c r="K25" s="60"/>
+      <c r="K25" s="62"/>
     </row>
     <row r="27" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="62" t="s">
+      <c r="A28" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="B28" s="62"/>
+      <c r="B28" s="56"/>
     </row>
     <row r="29" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18">
@@ -6350,10 +6399,10 @@
       <c r="A31" s="44">
         <v>1</v>
       </c>
-      <c r="E31" s="55" t="s">
+      <c r="E31" s="57" t="s">
         <v>252</v>
       </c>
-      <c r="F31" s="55"/>
+      <c r="F31" s="57"/>
     </row>
     <row r="32" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D32" s="44">
@@ -6372,14 +6421,14 @@
       </c>
     </row>
     <row r="34" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="60" t="s">
+      <c r="C34" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="D34" s="60"/>
-      <c r="G34" s="60" t="s">
+      <c r="D34" s="62"/>
+      <c r="G34" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="H34" s="60"/>
+      <c r="H34" s="62"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="s">
@@ -6409,14 +6458,14 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="59" t="s">
+      <c r="A38" s="55" t="s">
         <v>242</v>
       </c>
-      <c r="B38" s="59"/>
-      <c r="G38" s="56" t="s">
+      <c r="B38" s="55"/>
+      <c r="G38" s="58" t="s">
         <v>239</v>
       </c>
-      <c r="H38" s="56"/>
+      <c r="H38" s="58"/>
       <c r="I38" s="44">
         <v>1</v>
       </c>
@@ -6437,10 +6486,10 @@
       <c r="H39">
         <v>1</v>
       </c>
-      <c r="J39" s="60" t="s">
+      <c r="J39" s="62" t="s">
         <v>267</v>
       </c>
-      <c r="K39" s="60"/>
+      <c r="K39" s="62"/>
       <c r="L39" s="44" t="s">
         <v>243</v>
       </c>
@@ -6494,20 +6543,20 @@
       <c r="E43" t="s">
         <v>243</v>
       </c>
-      <c r="K43" s="62" t="s">
+      <c r="K43" s="56" t="s">
         <v>265</v>
       </c>
-      <c r="L43" s="62"/>
+      <c r="L43" s="56"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="60" t="s">
+      <c r="A44" s="62" t="s">
         <v>241</v>
       </c>
-      <c r="B44" s="60"/>
-      <c r="E44" s="58" t="s">
+      <c r="B44" s="62"/>
+      <c r="E44" s="60" t="s">
         <v>244</v>
       </c>
-      <c r="F44" s="58"/>
+      <c r="F44" s="60"/>
       <c r="K44" t="s">
         <v>243</v>
       </c>
@@ -6531,14 +6580,14 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="54" t="s">
+      <c r="A51" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="B51" s="54"/>
-      <c r="E51" s="57" t="s">
+      <c r="B51" s="61"/>
+      <c r="E51" s="59" t="s">
         <v>228</v>
       </c>
-      <c r="F51" s="57"/>
+      <c r="F51" s="59"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52">

</xml_diff>

<commit_message>
Docs: Modificación de datos
</commit_message>
<xml_diff>
--- a/Primer_Trimestres/Nomalizacion/correccion/Normalización .xlsx
+++ b/Primer_Trimestres/Nomalizacion/correccion/Normalización .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d01d89a1400d5043/Documentos/FARMIFARMACY/Docs excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMBIENTE\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{5D5CD52F-53E4-4F0F-B9B6-38621EE8DA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD59913C-B014-4078-B1D8-E39275E402CF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104EEF89-F2B3-49DC-9324-F38107CAC097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="3" activeTab="7" xr2:uid="{EB7CC955-6B47-4A67-9DA5-CC93A65E4CC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="7" xr2:uid="{EB7CC955-6B47-4A67-9DA5-CC93A65E4CC7}"/>
   </bookViews>
   <sheets>
     <sheet name="cliente" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="303">
   <si>
     <t>identificacion</t>
   </si>
@@ -754,12 +754,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>COTIZACIÓN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Id_Cotización </t>
-  </si>
-  <si>
     <t>Desc_T-doc</t>
   </si>
   <si>
@@ -850,13 +844,103 @@
     <t>USUARIO-PRODUCTO</t>
   </si>
   <si>
-    <t xml:space="preserve">USUARIO-COTIZACIÓN </t>
-  </si>
-  <si>
     <t>USUARIO-ROL</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cod_venta </t>
+  </si>
+  <si>
+    <t>CARRO DE COMPRAS</t>
+  </si>
+  <si>
+    <t>Item_producto</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Valor SubTotal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cod_Carro </t>
+  </si>
+  <si>
+    <t>V_001</t>
+  </si>
+  <si>
+    <t>V_002</t>
+  </si>
+  <si>
+    <t>V_003</t>
+  </si>
+  <si>
+    <t>V_004</t>
+  </si>
+  <si>
+    <t>V_005</t>
+  </si>
+  <si>
+    <t>V_006</t>
+  </si>
+  <si>
+    <t>V_007</t>
+  </si>
+  <si>
+    <t>V_008</t>
+  </si>
+  <si>
+    <t>V_009</t>
+  </si>
+  <si>
+    <t>V_010</t>
+  </si>
+  <si>
+    <t>V_011</t>
+  </si>
+  <si>
+    <t>V_012</t>
+  </si>
+  <si>
+    <t>V_013</t>
+  </si>
+  <si>
+    <t>V_014</t>
+  </si>
+  <si>
+    <t>V_015</t>
+  </si>
+  <si>
+    <t>V_016</t>
+  </si>
+  <si>
+    <t>V_017</t>
+  </si>
+  <si>
+    <t>V_018</t>
+  </si>
+  <si>
+    <t>V_019</t>
+  </si>
+  <si>
+    <t>V_020</t>
+  </si>
+  <si>
+    <t>VENTA-USUARIO</t>
+  </si>
+  <si>
+    <t>USUARIO-CARRO DE COMPRAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id_Carro </t>
+  </si>
+  <si>
+    <t>VENTA-CARRO DE COMPRAS</t>
+  </si>
+  <si>
+    <t>VENTA</t>
   </si>
 </sst>
 </file>
@@ -864,12 +948,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.000_-;\-&quot;$&quot;\ * #,##0.000_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;* #,##0.000_-;\-&quot;$&quot;* #,##0.000_-;_-&quot;$&quot;* &quot;-&quot;???_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;???_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="0000"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0.000_-;\-&quot;$&quot;\ * #,##0.000_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;* #,##0.000_-;\-&quot;$&quot;* #,##0.000_-;_-&quot;$&quot;* &quot;-&quot;???_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;???_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -914,7 +998,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1029,8 +1113,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1101,35 +1191,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
@@ -1137,7 +1214,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1147,14 +1224,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1199,13 +1276,13 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1220,7 +1297,7 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="15" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1230,6 +1307,67 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1237,6 +1375,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1254,74 +1398,35 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1611,23 +1716,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1095375</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="30" name="Conector recto 29">
+        <xdr:cNvPr id="10" name="Conector recto 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CD1FD81-1E5C-437A-BCB7-F15A91CBFEBB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3773BE0-2CA0-48CD-BC43-3663B6E9E7A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1635,14 +1740,14 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7181850" y="10877550"/>
-          <a:ext cx="923925" cy="733425"/>
+          <a:off x="7191375" y="10868025"/>
+          <a:ext cx="3886200" cy="1152525"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="28575">
-          <a:prstDash val="solid"/>
+          <a:prstDash val="dash"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -1664,32 +1769,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="33" name="Conector recto 32">
+        <xdr:cNvPr id="12" name="Conector recto 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD035D81-B7ED-4CC0-B4D8-860ACCB87DAF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{870F02DC-6715-4023-B041-67A2854FA8B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10210800" y="11610975"/>
-          <a:ext cx="876300" cy="400050"/>
+        <a:xfrm flipV="1">
+          <a:off x="12153900" y="12230100"/>
+          <a:ext cx="19050" cy="1457325"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2313,7 +2418,7 @@
       </c>
       <c r="D2" s="15">
         <f ca="1">NOW()</f>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E2" s="15">
         <v>44673.458333333336</v>
@@ -2331,7 +2436,7 @@
       </c>
       <c r="D3" s="15">
         <f t="shared" ref="D3:D20" ca="1" si="0">NOW()</f>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E3" s="15">
         <v>44674.458333333336</v>
@@ -2349,7 +2454,7 @@
       </c>
       <c r="D4" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E4" s="15">
         <v>44675.458333333336</v>
@@ -2367,7 +2472,7 @@
       </c>
       <c r="D5" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E5" s="15">
         <v>44676.458333333336</v>
@@ -2385,7 +2490,7 @@
       </c>
       <c r="D6" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E6" s="15">
         <v>44677.458333333336</v>
@@ -2403,7 +2508,7 @@
       </c>
       <c r="D7" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E7" s="15">
         <v>44678.458333333336</v>
@@ -2421,7 +2526,7 @@
       </c>
       <c r="D8" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E8" s="15">
         <v>44679.458333333336</v>
@@ -2439,7 +2544,7 @@
       </c>
       <c r="D9" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E9" s="15">
         <v>44680.458333333336</v>
@@ -2457,7 +2562,7 @@
       </c>
       <c r="D10" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E10" s="15">
         <v>44681.458333333336</v>
@@ -2475,7 +2580,7 @@
       </c>
       <c r="D11" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E11" s="15">
         <v>44682.458333333336</v>
@@ -2493,7 +2598,7 @@
       </c>
       <c r="D12" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E12" s="15">
         <v>44683.458333333336</v>
@@ -2511,7 +2616,7 @@
       </c>
       <c r="D13" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E13" s="15">
         <v>44684.458333333336</v>
@@ -2529,7 +2634,7 @@
       </c>
       <c r="D14" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E14" s="15">
         <v>44685.458333333336</v>
@@ -2547,7 +2652,7 @@
       </c>
       <c r="D15" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E15" s="15">
         <v>44686.458333333336</v>
@@ -2565,7 +2670,7 @@
       </c>
       <c r="D16" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E16" s="15">
         <v>44687.458333333336</v>
@@ -2583,7 +2688,7 @@
       </c>
       <c r="D17" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E17" s="15">
         <v>44688.458333333336</v>
@@ -2601,7 +2706,7 @@
       </c>
       <c r="D18" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E18" s="15">
         <v>44689.458333333336</v>
@@ -2619,7 +2724,7 @@
       </c>
       <c r="D19" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E19" s="15">
         <v>44690.458333333336</v>
@@ -2637,7 +2742,7 @@
       </c>
       <c r="D20" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
       <c r="E20" s="15">
         <v>44691.458333333336</v>
@@ -2836,63 +2941,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="49">
+      <c r="B1" s="73"/>
+      <c r="C1" s="72">
         <v>1192831945</v>
       </c>
-      <c r="D1" s="49"/>
+      <c r="D1" s="72"/>
       <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="5">
         <f ca="1">NOW()</f>
-        <v>44372.768375462962</v>
+        <v>44411.600464236108</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="51" t="s">
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="51"/>
+      <c r="F2" s="74"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="49">
+      <c r="B4" s="72">
         <v>3172727783</v>
       </c>
-      <c r="C4" s="49"/>
+      <c r="C4" s="72"/>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="49"/>
+      <c r="F4" s="72"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -3085,39 +3190,39 @@
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49" t="s">
+      <c r="B16" s="72"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="49"/>
+      <c r="E16" s="72"/>
       <c r="F16" s="6">
         <v>389</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49" t="s">
+      <c r="A17" s="72"/>
+      <c r="B17" s="72"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="49"/>
+      <c r="E17" s="72"/>
       <c r="F17" s="6">
         <v>73.91</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49" t="s">
+      <c r="A18" s="72"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="49"/>
+      <c r="E18" s="72"/>
       <c r="F18" s="6">
         <v>462.90999999999997</v>
       </c>
@@ -3162,7 +3267,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3171,6 +3276,7 @@
     <col min="2" max="2" width="36.140625" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="5" max="5" width="42.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="34" customWidth="1"/>
     <col min="12" max="12" width="15.85546875" customWidth="1"/>
     <col min="16" max="16" width="14.85546875" customWidth="1"/>
@@ -3781,8 +3887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B9B3C5C-ADFC-4BC2-AC69-E82DBE3B9792}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView topLeftCell="J4" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4657,8 +4763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{154A3EB2-7D84-4648-B4B7-AFD12D379634}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46:I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4711,10 +4817,10 @@
         <v>134</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J1" s="30" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -4741,7 +4847,7 @@
         <v>46</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J2" s="31" t="s">
         <v>131</v>
@@ -4773,7 +4879,7 @@
         <v>50</v>
       </c>
       <c r="I3" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J3" s="31" t="s">
         <v>131</v>
@@ -4805,7 +4911,7 @@
         <v>53</v>
       </c>
       <c r="I4" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J4" s="31" t="s">
         <v>131</v>
@@ -4837,7 +4943,7 @@
         <v>57</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J5" s="31" t="s">
         <v>131</v>
@@ -4869,7 +4975,7 @@
         <v>9</v>
       </c>
       <c r="I6" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J6" s="31" t="s">
         <v>131</v>
@@ -4901,7 +5007,7 @@
         <v>63</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J7" s="31" t="s">
         <v>131</v>
@@ -4933,7 +5039,7 @@
         <v>67</v>
       </c>
       <c r="I8" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J8" s="31" t="s">
         <v>131</v>
@@ -4965,7 +5071,7 @@
         <v>71</v>
       </c>
       <c r="I9" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J9" s="31" t="s">
         <v>131</v>
@@ -4997,7 +5103,7 @@
         <v>75</v>
       </c>
       <c r="I10" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J10" s="31" t="s">
         <v>131</v>
@@ -5029,7 +5135,7 @@
         <v>79</v>
       </c>
       <c r="I11" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J11" s="31" t="s">
         <v>131</v>
@@ -5055,10 +5161,10 @@
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
       <c r="I12" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J12" s="31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -5079,10 +5185,10 @@
       <c r="G13" s="30"/>
       <c r="H13" s="30"/>
       <c r="I13" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -5101,10 +5207,10 @@
       <c r="G14" s="30"/>
       <c r="H14" s="30"/>
       <c r="I14" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J14" s="31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -5127,10 +5233,10 @@
       <c r="G15" s="30"/>
       <c r="H15" s="30"/>
       <c r="I15" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J15" s="31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -5151,10 +5257,10 @@
       <c r="G16" s="30"/>
       <c r="H16" s="30"/>
       <c r="I16" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J16" s="31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -5177,10 +5283,10 @@
       <c r="G17" s="30"/>
       <c r="H17" s="30"/>
       <c r="I17" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J17" s="31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -5201,10 +5307,10 @@
       <c r="G18" s="30"/>
       <c r="H18" s="30"/>
       <c r="I18" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J18" s="31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -5223,10 +5329,10 @@
       <c r="G19" s="30"/>
       <c r="H19" s="30"/>
       <c r="I19" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J19" s="31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -5249,10 +5355,10 @@
       <c r="G20" s="30"/>
       <c r="H20" s="30"/>
       <c r="I20" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J20" s="31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -5275,42 +5381,48 @@
       <c r="G21" s="30"/>
       <c r="H21" s="30"/>
       <c r="I21" s="31" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J21" s="31" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="61" t="s">
-        <v>267</v>
-      </c>
-      <c r="B22" s="61"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
+      <c r="A22" s="75" t="s">
+        <v>265</v>
+      </c>
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="75"/>
+      <c r="J22" s="75"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="43" t="s">
-        <v>241</v>
+        <v>277</v>
       </c>
       <c r="B24" s="41" t="s">
         <v>135</v>
       </c>
       <c r="C24" s="44" t="s">
-        <v>142</v>
-      </c>
-      <c r="D24" s="60"/>
+        <v>276</v>
+      </c>
+      <c r="D24" s="50"/>
       <c r="E24" s="33" t="s">
         <v>231</v>
       </c>
       <c r="F24" s="34" t="s">
         <v>229</v>
+      </c>
+      <c r="H24" s="64" t="s">
+        <v>272</v>
+      </c>
+      <c r="I24" s="65" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -5321,13 +5433,19 @@
         <v>44228</v>
       </c>
       <c r="C25" s="45">
-        <v>129</v>
+        <v>389</v>
       </c>
       <c r="E25" s="33" t="s">
         <v>232</v>
       </c>
       <c r="F25" s="47">
         <v>1234</v>
+      </c>
+      <c r="H25" s="64" t="s">
+        <v>278</v>
+      </c>
+      <c r="I25" s="66">
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -5338,13 +5456,19 @@
         <v>44229</v>
       </c>
       <c r="C26" s="45">
-        <v>76</v>
+        <v>389</v>
       </c>
       <c r="E26" s="33" t="s">
         <v>233</v>
       </c>
       <c r="F26" s="47">
         <v>2876</v>
+      </c>
+      <c r="H26" s="64" t="s">
+        <v>279</v>
+      </c>
+      <c r="I26" s="66">
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -5355,13 +5479,19 @@
         <v>44230</v>
       </c>
       <c r="C27" s="45">
-        <v>16</v>
+        <v>389</v>
       </c>
       <c r="E27" s="33" t="s">
         <v>234</v>
       </c>
       <c r="F27" s="47">
         <v>8744</v>
+      </c>
+      <c r="H27" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="I27" s="66">
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -5372,13 +5502,19 @@
         <v>44231</v>
       </c>
       <c r="C28" s="45">
-        <v>18</v>
+        <v>389</v>
       </c>
       <c r="E28" s="33" t="s">
         <v>235</v>
       </c>
       <c r="F28" s="47">
         <v>3978</v>
+      </c>
+      <c r="H28" s="64" t="s">
+        <v>281</v>
+      </c>
+      <c r="I28" s="66">
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -5389,13 +5525,19 @@
         <v>44232</v>
       </c>
       <c r="C29" s="45">
-        <v>14</v>
+        <v>389</v>
       </c>
       <c r="E29" s="33" t="s">
         <v>236</v>
       </c>
       <c r="F29" s="47">
         <v>2938</v>
+      </c>
+      <c r="H29" s="64" t="s">
+        <v>282</v>
+      </c>
+      <c r="I29" s="66">
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -5406,13 +5548,19 @@
         <v>44233</v>
       </c>
       <c r="C30" s="45">
-        <v>46</v>
+        <v>389</v>
       </c>
       <c r="E30" s="33" t="s">
         <v>237</v>
       </c>
       <c r="F30" s="47">
         <v>4937</v>
+      </c>
+      <c r="H30" s="64" t="s">
+        <v>283</v>
+      </c>
+      <c r="I30" s="66">
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -5423,13 +5571,19 @@
         <v>44234</v>
       </c>
       <c r="C31" s="45">
-        <v>90</v>
+        <v>389</v>
       </c>
       <c r="E31" s="33" t="s">
         <v>238</v>
       </c>
       <c r="F31" s="47">
         <v>8736</v>
+      </c>
+      <c r="H31" s="64" t="s">
+        <v>284</v>
+      </c>
+      <c r="I31" s="66">
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -5440,14 +5594,20 @@
         <v>44235</v>
       </c>
       <c r="C32" s="45">
+        <v>389</v>
+      </c>
+      <c r="E32" s="79" t="s">
+        <v>228</v>
+      </c>
+      <c r="F32" s="79"/>
+      <c r="H32" s="64" t="s">
+        <v>285</v>
+      </c>
+      <c r="I32" s="66">
         <v>129</v>
       </c>
-      <c r="E32" s="54" t="s">
-        <v>228</v>
-      </c>
-      <c r="F32" s="54"/>
-    </row>
-    <row r="33" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="40">
         <v>9</v>
       </c>
@@ -5455,10 +5615,16 @@
         <v>44236</v>
       </c>
       <c r="C33" s="45">
+        <v>389</v>
+      </c>
+      <c r="H33" s="64" t="s">
+        <v>286</v>
+      </c>
+      <c r="I33" s="66">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="40">
         <v>10</v>
       </c>
@@ -5466,20 +5632,39 @@
         <v>44237</v>
       </c>
       <c r="C34" s="45">
+        <v>389</v>
+      </c>
+      <c r="H34" s="64" t="s">
+        <v>287</v>
+      </c>
+      <c r="I34" s="66">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="55" t="s">
-        <v>240</v>
-      </c>
-      <c r="B35" s="55"/>
-      <c r="C35" s="55"/>
-    </row>
-    <row r="36" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="80" t="s">
+        <v>273</v>
+      </c>
+      <c r="B35" s="80"/>
+      <c r="C35" s="80"/>
+      <c r="H35" s="64" t="s">
+        <v>287</v>
+      </c>
+      <c r="I35" s="66">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="64" t="s">
+        <v>288</v>
+      </c>
+      <c r="I36" s="66">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="35" t="s">
-        <v>139</v>
+        <v>274</v>
       </c>
       <c r="B37" s="37" t="s">
         <v>138</v>
@@ -5491,10 +5676,16 @@
         <v>141</v>
       </c>
       <c r="E37" s="37" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="H37" s="64" t="s">
+        <v>289</v>
+      </c>
+      <c r="I37" s="66">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="35" t="s">
         <v>16</v>
       </c>
@@ -5508,10 +5699,16 @@
         <v>43</v>
       </c>
       <c r="E38" s="36" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="H38" s="64" t="s">
+        <v>290</v>
+      </c>
+      <c r="I38" s="66">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="35" t="s">
         <v>18</v>
       </c>
@@ -5525,10 +5722,16 @@
         <v>76</v>
       </c>
       <c r="E39" s="36" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+      <c r="H39" s="64" t="s">
+        <v>291</v>
+      </c>
+      <c r="I39" s="66">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="35" t="s">
         <v>20</v>
       </c>
@@ -5542,10 +5745,16 @@
         <v>8</v>
       </c>
       <c r="E40" s="36" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="H40" s="64" t="s">
+        <v>292</v>
+      </c>
+      <c r="I40" s="66">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="35" t="s">
         <v>22</v>
       </c>
@@ -5559,10 +5768,16 @@
         <v>6</v>
       </c>
       <c r="E41" s="36" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+      <c r="H41" s="64" t="s">
+        <v>293</v>
+      </c>
+      <c r="I41" s="66">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="35" t="s">
         <v>24</v>
       </c>
@@ -5576,10 +5791,16 @@
         <v>7</v>
       </c>
       <c r="E42" s="36" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+      <c r="H42" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="I42" s="66">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="35" t="s">
         <v>26</v>
       </c>
@@ -5593,10 +5814,16 @@
         <v>23</v>
       </c>
       <c r="E43" s="36" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="H43" s="64" t="s">
+        <v>295</v>
+      </c>
+      <c r="I43" s="66">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="35" t="s">
         <v>28</v>
       </c>
@@ -5610,92 +5837,111 @@
         <v>30</v>
       </c>
       <c r="E44" s="36" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="56" t="s">
+        <v>262</v>
+      </c>
+      <c r="H44" s="64" t="s">
+        <v>296</v>
+      </c>
+      <c r="I44" s="66">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="81"/>
+      <c r="C45" s="81"/>
+      <c r="D45" s="81"/>
+      <c r="E45" s="81"/>
+      <c r="H45" s="64" t="s">
+        <v>297</v>
+      </c>
+      <c r="I45" s="66">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H46" s="76" t="s">
+        <v>302</v>
+      </c>
+      <c r="I46" s="76"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="39" t="s">
         <v>230</v>
       </c>
       <c r="B47" s="33" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D47" s="43" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E47" s="46" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="29" t="s">
         <v>178</v>
       </c>
       <c r="B48" s="33" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D48" s="43" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E48" s="46" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="39" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B49" s="33" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D49" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E49" s="46" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B50" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="D50" s="43" t="s">
+        <v>254</v>
+      </c>
+      <c r="E50" s="46" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="78" t="s">
         <v>246</v>
       </c>
-      <c r="D50" s="43" t="s">
-        <v>256</v>
-      </c>
-      <c r="E50" s="46" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="53" t="s">
-        <v>248</v>
-      </c>
-      <c r="B51" s="53"/>
-      <c r="D51" s="52" t="s">
-        <v>269</v>
-      </c>
-      <c r="E51" s="52"/>
+      <c r="B51" s="78"/>
+      <c r="D51" s="77" t="s">
+        <v>267</v>
+      </c>
+      <c r="E51" s="77"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A22:J22"/>
+    <mergeCell ref="H46:I46"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A45:E45"/>
-    <mergeCell ref="A22:J22"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -5719,8 +5965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C15CDDD0-1EC6-46EB-86DD-BB5C7073D9F7}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5761,14 +6007,14 @@
         <v>167</v>
       </c>
       <c r="K1" s="43" t="s">
-        <v>241</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="29">
         <v>1013576811</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="52" t="s">
         <v>178</v>
       </c>
       <c r="D2" s="35" t="s">
@@ -5794,7 +6040,7 @@
       <c r="A3" s="29">
         <v>1001096125</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="52" t="s">
         <v>178</v>
       </c>
       <c r="D3" s="35" t="s">
@@ -5820,7 +6066,7 @@
       <c r="A4" s="29">
         <v>1012316243</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="52" t="s">
         <v>178</v>
       </c>
       <c r="D4" s="35" t="s">
@@ -5846,7 +6092,7 @@
       <c r="A5" s="29">
         <v>1016942358</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="52" t="s">
         <v>178</v>
       </c>
       <c r="D5" s="35" t="s">
@@ -5872,7 +6118,7 @@
       <c r="A6" s="29">
         <v>1192831945</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="52" t="s">
         <v>178</v>
       </c>
       <c r="D6" s="35" t="s">
@@ -5898,7 +6144,7 @@
       <c r="A7" s="29">
         <v>1016943117</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="52" t="s">
         <v>178</v>
       </c>
       <c r="D7" s="35" t="s">
@@ -5924,7 +6170,7 @@
       <c r="A8" s="29">
         <v>1010051342</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="52" t="s">
         <v>178</v>
       </c>
       <c r="D8" s="35" t="s">
@@ -5950,7 +6196,7 @@
       <c r="A9" s="29">
         <v>1006051207</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="52" t="s">
         <v>178</v>
       </c>
       <c r="D9" s="35" t="s">
@@ -5976,7 +6222,7 @@
       <c r="A10" s="29">
         <v>1014176160</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="52" t="s">
         <v>178</v>
       </c>
       <c r="D10" s="35" t="s">
@@ -5999,10 +6245,10 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="62">
+      <c r="A11" s="51">
         <v>1000350620</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="52" t="s">
         <v>178</v>
       </c>
       <c r="D11" s="35" t="s">
@@ -6028,27 +6274,27 @@
       <c r="A12" s="39">
         <v>1016841206</v>
       </c>
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="52" t="s">
         <v>178</v>
       </c>
-      <c r="D12" s="57" t="s">
-        <v>249</v>
-      </c>
-      <c r="E12" s="57"/>
-      <c r="G12" s="57" t="s">
-        <v>271</v>
-      </c>
-      <c r="H12" s="57"/>
-      <c r="J12" s="57" t="s">
-        <v>272</v>
-      </c>
-      <c r="K12" s="57"/>
+      <c r="D12" s="83" t="s">
+        <v>247</v>
+      </c>
+      <c r="E12" s="83"/>
+      <c r="G12" s="83" t="s">
+        <v>269</v>
+      </c>
+      <c r="H12" s="83"/>
+      <c r="J12" s="83" t="s">
+        <v>299</v>
+      </c>
+      <c r="K12" s="83"/>
     </row>
     <row r="13" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="39">
         <v>1003275748</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="52" t="s">
         <v>178</v>
       </c>
       <c r="G13"/>
@@ -6061,7 +6307,7 @@
       <c r="A14" s="39">
         <v>1011153857</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="52" t="s">
         <v>178</v>
       </c>
     </row>
@@ -6069,7 +6315,7 @@
       <c r="A15" s="39">
         <v>1026238784</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="52" t="s">
         <v>178</v>
       </c>
     </row>
@@ -6077,127 +6323,235 @@
       <c r="A16" s="39">
         <v>1011752470</v>
       </c>
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="52" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="39">
         <v>1000016762</v>
       </c>
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="52" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="39">
         <v>1021928374</v>
       </c>
-      <c r="B18" s="63" t="s">
+      <c r="B18" s="52" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="39">
         <v>1015159424</v>
       </c>
-      <c r="B19" s="63" t="s">
+      <c r="B19" s="52" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="39">
         <v>1009812763</v>
       </c>
-      <c r="B20" s="63" t="s">
+      <c r="B20" s="52" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="39">
         <v>10281927364</v>
       </c>
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="52" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="57" t="s">
-        <v>270</v>
-      </c>
-      <c r="B22" s="57"/>
-    </row>
-    <row r="23" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="83" t="s">
+        <v>268</v>
+      </c>
+      <c r="B22" s="83"/>
+    </row>
+    <row r="23" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>167</v>
       </c>
       <c r="B24" s="43" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+      <c r="D24" s="64" t="s">
+        <v>272</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="G24" s="64" t="s">
+        <v>272</v>
+      </c>
+      <c r="H24" s="43" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29">
         <v>1013576811</v>
       </c>
       <c r="B25" s="43" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="D25" s="64" t="s">
+        <v>278</v>
+      </c>
+      <c r="E25" s="29">
+        <v>1013576811</v>
+      </c>
+      <c r="G25" s="64" t="s">
+        <v>278</v>
+      </c>
+      <c r="H25" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <v>1001096125</v>
       </c>
       <c r="B26" s="43" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="D26" s="64" t="s">
+        <v>279</v>
+      </c>
+      <c r="E26" s="29">
+        <v>1001096125</v>
+      </c>
+      <c r="G26" s="64" t="s">
+        <v>279</v>
+      </c>
+      <c r="H26" s="40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <v>1012316243</v>
       </c>
       <c r="B27" s="43" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="D27" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="E27" s="29">
+        <v>1012316243</v>
+      </c>
+      <c r="G27" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="H27" s="40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>1016942358</v>
       </c>
       <c r="B28" s="43" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="D28" s="64" t="s">
+        <v>281</v>
+      </c>
+      <c r="E28" s="29">
+        <v>1016942358</v>
+      </c>
+      <c r="G28" s="64" t="s">
+        <v>281</v>
+      </c>
+      <c r="H28" s="40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
         <v>1192831945</v>
       </c>
       <c r="B29" s="43" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="D29" s="64" t="s">
+        <v>282</v>
+      </c>
+      <c r="E29" s="29">
+        <v>1192831945</v>
+      </c>
+      <c r="G29" s="64" t="s">
+        <v>282</v>
+      </c>
+      <c r="H29" s="40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>1016943117</v>
       </c>
       <c r="B30" s="43" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="D30" s="64" t="s">
+        <v>283</v>
+      </c>
+      <c r="E30" s="29">
+        <v>1016943117</v>
+      </c>
+      <c r="G30" s="64" t="s">
+        <v>283</v>
+      </c>
+      <c r="H30" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
         <v>1010051342</v>
       </c>
       <c r="B31" s="43" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="D31" s="64" t="s">
+        <v>284</v>
+      </c>
+      <c r="E31" s="29">
+        <v>1010051342</v>
+      </c>
+      <c r="G31" s="64" t="s">
+        <v>284</v>
+      </c>
+      <c r="H31" s="40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>1006051207</v>
       </c>
       <c r="B32" s="43" t="s">
-        <v>256</v>
+        <v>254</v>
+      </c>
+      <c r="D32" s="64" t="s">
+        <v>285</v>
+      </c>
+      <c r="E32" s="29">
+        <v>1006051207</v>
+      </c>
+      <c r="G32" s="64" t="s">
+        <v>285</v>
+      </c>
+      <c r="H32" s="40">
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -6205,15 +6559,39 @@
         <v>1014176160</v>
       </c>
       <c r="B33" s="43" t="s">
-        <v>256</v>
+        <v>254</v>
+      </c>
+      <c r="D33" s="64" t="s">
+        <v>286</v>
+      </c>
+      <c r="E33" s="29">
+        <v>1014176160</v>
+      </c>
+      <c r="G33" s="64" t="s">
+        <v>286</v>
+      </c>
+      <c r="H33" s="40">
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="62">
+      <c r="A34" s="51">
         <v>1000350620</v>
       </c>
       <c r="B34" s="43" t="s">
-        <v>256</v>
+        <v>254</v>
+      </c>
+      <c r="D34" s="64" t="s">
+        <v>287</v>
+      </c>
+      <c r="E34" s="51">
+        <v>1000350620</v>
+      </c>
+      <c r="G34" s="64" t="s">
+        <v>287</v>
+      </c>
+      <c r="H34" s="40">
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -6221,7 +6599,19 @@
         <v>1016841206</v>
       </c>
       <c r="B35" s="43" t="s">
-        <v>254</v>
+        <v>252</v>
+      </c>
+      <c r="D35" s="64" t="s">
+        <v>288</v>
+      </c>
+      <c r="E35" s="39">
+        <v>1016841206</v>
+      </c>
+      <c r="G35" s="64" t="s">
+        <v>288</v>
+      </c>
+      <c r="H35" s="40">
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -6229,7 +6619,19 @@
         <v>1003275748</v>
       </c>
       <c r="B36" s="43" t="s">
-        <v>254</v>
+        <v>252</v>
+      </c>
+      <c r="D36" s="64" t="s">
+        <v>289</v>
+      </c>
+      <c r="E36" s="39">
+        <v>1003275748</v>
+      </c>
+      <c r="G36" s="64" t="s">
+        <v>289</v>
+      </c>
+      <c r="H36" s="40">
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -6237,7 +6639,19 @@
         <v>1011153857</v>
       </c>
       <c r="B37" s="43" t="s">
-        <v>254</v>
+        <v>252</v>
+      </c>
+      <c r="D37" s="64" t="s">
+        <v>290</v>
+      </c>
+      <c r="E37" s="39">
+        <v>1011153857</v>
+      </c>
+      <c r="G37" s="64" t="s">
+        <v>290</v>
+      </c>
+      <c r="H37" s="40">
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -6245,7 +6659,19 @@
         <v>1026238784</v>
       </c>
       <c r="B38" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
+      </c>
+      <c r="D38" s="64" t="s">
+        <v>291</v>
+      </c>
+      <c r="E38" s="39">
+        <v>1026238784</v>
+      </c>
+      <c r="G38" s="64" t="s">
+        <v>291</v>
+      </c>
+      <c r="H38" s="40">
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -6253,7 +6679,19 @@
         <v>1011752470</v>
       </c>
       <c r="B39" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
+      </c>
+      <c r="D39" s="64" t="s">
+        <v>292</v>
+      </c>
+      <c r="E39" s="39">
+        <v>1011752470</v>
+      </c>
+      <c r="G39" s="64" t="s">
+        <v>292</v>
+      </c>
+      <c r="H39" s="40">
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -6261,7 +6699,19 @@
         <v>1000016762</v>
       </c>
       <c r="B40" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
+      </c>
+      <c r="D40" s="64" t="s">
+        <v>293</v>
+      </c>
+      <c r="E40" s="39">
+        <v>1000016762</v>
+      </c>
+      <c r="G40" s="64" t="s">
+        <v>293</v>
+      </c>
+      <c r="H40" s="40">
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -6269,7 +6719,19 @@
         <v>1021928374</v>
       </c>
       <c r="B41" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
+      </c>
+      <c r="D41" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="E41" s="39">
+        <v>1021928374</v>
+      </c>
+      <c r="G41" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="H41" s="40">
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -6277,7 +6739,19 @@
         <v>1015159424</v>
       </c>
       <c r="B42" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
+      </c>
+      <c r="D42" s="64" t="s">
+        <v>295</v>
+      </c>
+      <c r="E42" s="39">
+        <v>1015159424</v>
+      </c>
+      <c r="G42" s="64" t="s">
+        <v>295</v>
+      </c>
+      <c r="H42" s="40">
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -6285,7 +6759,19 @@
         <v>1009812763</v>
       </c>
       <c r="B43" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
+      </c>
+      <c r="D43" s="64" t="s">
+        <v>296</v>
+      </c>
+      <c r="E43" s="39">
+        <v>1009812763</v>
+      </c>
+      <c r="G43" s="64" t="s">
+        <v>296</v>
+      </c>
+      <c r="H43" s="40">
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -6293,20 +6779,40 @@
         <v>10281927364</v>
       </c>
       <c r="B44" s="43" t="s">
-        <v>255</v>
+        <v>253</v>
+      </c>
+      <c r="D44" s="64" t="s">
+        <v>297</v>
+      </c>
+      <c r="E44" s="39">
+        <v>10281927364</v>
+      </c>
+      <c r="G44" s="64" t="s">
+        <v>297</v>
+      </c>
+      <c r="H44" s="40">
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="57" t="s">
-        <v>273</v>
-      </c>
-      <c r="B45" s="57"/>
+      <c r="A45" s="83" t="s">
+        <v>270</v>
+      </c>
+      <c r="B45" s="83"/>
+      <c r="D45" s="83" t="s">
+        <v>298</v>
+      </c>
+      <c r="E45" s="83"/>
+      <c r="G45" s="83" t="s">
+        <v>301</v>
+      </c>
+      <c r="H45" s="83"/>
     </row>
     <row r="47" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="71">
+      <c r="C47" s="56">
         <v>1</v>
       </c>
-      <c r="L47" s="75" t="s">
+      <c r="L47" s="59" t="s">
         <v>239</v>
       </c>
     </row>
@@ -6321,63 +6827,63 @@
       </c>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C49" s="69">
+      <c r="C49" s="55">
         <v>1</v>
       </c>
-      <c r="F49" s="59"/>
+      <c r="F49" s="49"/>
       <c r="I49" s="18"/>
       <c r="J49" s="18"/>
-      <c r="K49" s="64"/>
-      <c r="L49" s="68" t="s">
+      <c r="K49" s="53"/>
+      <c r="L49" s="54" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B50" s="70" t="s">
-        <v>248</v>
-      </c>
-      <c r="C50" s="70"/>
+      <c r="B50" s="86" t="s">
+        <v>246</v>
+      </c>
+      <c r="C50" s="86"/>
       <c r="I50" s="18"/>
       <c r="J50" s="18"/>
-      <c r="L50" s="74" t="s">
-        <v>269</v>
-      </c>
-      <c r="M50" s="52"/>
+      <c r="L50" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="M50" s="77"/>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="I51" s="18"/>
       <c r="J51" s="18"/>
-      <c r="L51" s="71">
+      <c r="L51" s="56">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C52" s="60"/>
-      <c r="I52" s="77" t="s">
-        <v>273</v>
-      </c>
-      <c r="J52" s="77"/>
+      <c r="C52" s="50"/>
+      <c r="I52" s="88" t="s">
+        <v>270</v>
+      </c>
+      <c r="J52" s="88"/>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I53" s="76" t="s">
+      <c r="I53" s="60" t="s">
         <v>239</v>
       </c>
-      <c r="J53" s="76" t="s">
+      <c r="J53" s="60" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F54" s="72" t="s">
+      <c r="F54" s="57" t="s">
         <v>239</v>
       </c>
-      <c r="G54" s="75" t="s">
+      <c r="G54" s="59" t="s">
         <v>239</v>
       </c>
       <c r="I54" s="18"/>
       <c r="J54" s="18"/>
     </row>
     <row r="55" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F55" s="73">
+      <c r="F55" s="58">
         <v>1</v>
       </c>
       <c r="G55" s="48" t="s">
@@ -6387,167 +6893,183 @@
       <c r="J55" s="18"/>
     </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F56" s="73" t="s">
+      <c r="F56" s="58" t="s">
         <v>239</v>
       </c>
-      <c r="G56" s="73">
+      <c r="G56" s="58">
         <v>1</v>
       </c>
-      <c r="H56" s="71">
+      <c r="H56" s="56">
         <v>1</v>
       </c>
       <c r="I56" s="18"/>
       <c r="J56" s="18"/>
     </row>
     <row r="57" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F57" s="58" t="s">
-        <v>267</v>
-      </c>
-      <c r="G57" s="58"/>
+      <c r="F57" s="90" t="s">
+        <v>265</v>
+      </c>
+      <c r="G57" s="90"/>
       <c r="I57" s="18"/>
       <c r="J57" s="18"/>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F58" s="78">
+      <c r="F58" s="69">
         <v>1</v>
       </c>
-      <c r="G58" s="79">
+      <c r="G58" s="61">
         <v>1</v>
       </c>
-      <c r="H58" s="71">
-        <v>1</v>
-      </c>
+      <c r="H58" s="68"/>
       <c r="I58" s="18"/>
       <c r="K58" s="18"/>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F59" s="78">
+      <c r="F59" s="69">
         <v>1</v>
       </c>
-      <c r="G59" s="79" t="s">
-        <v>239</v>
+      <c r="G59" s="62">
+        <v>1</v>
       </c>
       <c r="H59" s="18"/>
       <c r="I59" s="18"/>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F60" s="71">
+      <c r="F60" s="57">
         <v>1</v>
       </c>
-      <c r="G60" s="71" t="s">
+      <c r="G60" s="56">
+        <v>1</v>
+      </c>
+      <c r="H60" s="18"/>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C61" s="56" t="s">
         <v>239</v>
       </c>
-      <c r="H60" s="18"/>
-    </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C61" s="71" t="s">
+      <c r="H61" s="18"/>
+      <c r="I61" s="68"/>
+      <c r="J61" s="68"/>
+      <c r="L61" s="56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C62" s="61">
+        <v>1</v>
+      </c>
+      <c r="H62" s="18"/>
+      <c r="I62" s="89"/>
+      <c r="J62" s="89"/>
+      <c r="L62" s="63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C63" s="61" t="s">
         <v>239</v>
       </c>
-      <c r="H61" s="18"/>
-      <c r="I61" s="71" t="s">
-        <v>239</v>
-      </c>
-      <c r="J61" s="71" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C62" s="78">
+      <c r="H63" s="18"/>
+      <c r="I63" s="67"/>
+      <c r="L63" s="61">
         <v>1</v>
       </c>
-      <c r="H62" s="18"/>
-      <c r="I62" s="77" t="s">
-        <v>272</v>
-      </c>
-      <c r="J62" s="77"/>
-    </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C63" s="78" t="s">
-        <v>239</v>
-      </c>
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
-      <c r="L63" s="71">
-        <v>1</v>
-      </c>
     </row>
     <row r="64" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B64" s="67" t="s">
+      <c r="B64" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="C64" s="67"/>
+      <c r="C64" s="85"/>
       <c r="H64" s="18"/>
       <c r="I64" s="18"/>
-      <c r="L64" s="66" t="s">
-        <v>240</v>
-      </c>
-      <c r="M64" s="66"/>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C65" s="78">
+      <c r="L64" s="91" t="s">
+        <v>273</v>
+      </c>
+      <c r="M64" s="91"/>
+    </row>
+    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C65" s="61">
         <v>1</v>
       </c>
       <c r="F65" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="H65" s="18"/>
       <c r="I65" s="18"/>
-      <c r="L65" s="78" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C66" s="80" t="s">
+      <c r="L65" s="61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C66" s="62" t="s">
         <v>239</v>
       </c>
       <c r="H66" s="18"/>
       <c r="I66" s="18"/>
-      <c r="L66" s="78">
+      <c r="L66" s="61">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C67" s="71" t="s">
+    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C67" s="56" t="s">
         <v>239</v>
       </c>
-      <c r="L67" s="71" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B71" s="65" t="s">
+      <c r="L67" s="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L70" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B71" s="84" t="s">
         <v>228</v>
       </c>
-      <c r="C71" s="65"/>
-    </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C72" s="81">
+      <c r="C71" s="84"/>
+      <c r="L71" s="61">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C73" s="78">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C72" s="63">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C74" s="71">
+      <c r="L72" s="61">
         <v>1</v>
       </c>
     </row>
+    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C73" s="61">
+        <v>1</v>
+      </c>
+      <c r="L73" s="82" t="s">
+        <v>302</v>
+      </c>
+      <c r="M73" s="76"/>
+    </row>
+    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C74" s="56">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="16">
+    <mergeCell ref="L73:M73"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="G45:H45"/>
     <mergeCell ref="B71:C71"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="L50:M50"/>
     <mergeCell ref="I52:J52"/>
     <mergeCell ref="I62:J62"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A22:B22"/>
     <mergeCell ref="F57:G57"/>
     <mergeCell ref="L64:M64"/>
   </mergeCells>

</xml_diff>

<commit_message>
docs: Se modifican documentos
</commit_message>
<xml_diff>
--- a/Primer_Trimestres/Nomalizacion/correccion/Normalización .xlsx
+++ b/Primer_Trimestres/Nomalizacion/correccion/Normalización .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMBIENTE\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Heelen\OneDrive\Documentos\GitHub\farmifarmacy1.0\Primer_Trimestres\Nomalizacion\correccion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104EEF89-F2B3-49DC-9324-F38107CAC097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52862D3A-7303-448B-A1F3-EF6CA6C9E988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="7" xr2:uid="{EB7CC955-6B47-4A67-9DA5-CC93A65E4CC7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="3" activeTab="7" xr2:uid="{EB7CC955-6B47-4A67-9DA5-CC93A65E4CC7}"/>
   </bookViews>
   <sheets>
     <sheet name="cliente" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="303">
   <si>
     <t>identificacion</t>
   </si>
@@ -948,12 +948,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0.000_-;\-&quot;$&quot;\ * #,##0.000_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;* #,##0.000_-;\-&quot;$&quot;* #,##0.000_-;_-&quot;$&quot;* &quot;-&quot;???_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;???_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="0000"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.000_-;\-&quot;$&quot;\ * #,##0.000_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;* #,##0.000_-;\-&quot;$&quot;* #,##0.000_-;_-&quot;$&quot;* &quot;-&quot;???_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;???_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1194,7 +1194,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="92">
@@ -1204,9 +1204,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
@@ -1214,7 +1214,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1224,14 +1224,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1276,13 +1276,13 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1297,7 +1297,7 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="15" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1352,7 +1352,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -2418,7 +2418,7 @@
       </c>
       <c r="D2" s="15">
         <f ca="1">NOW()</f>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E2" s="15">
         <v>44673.458333333336</v>
@@ -2436,7 +2436,7 @@
       </c>
       <c r="D3" s="15">
         <f t="shared" ref="D3:D20" ca="1" si="0">NOW()</f>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E3" s="15">
         <v>44674.458333333336</v>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="D4" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E4" s="15">
         <v>44675.458333333336</v>
@@ -2472,7 +2472,7 @@
       </c>
       <c r="D5" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E5" s="15">
         <v>44676.458333333336</v>
@@ -2490,7 +2490,7 @@
       </c>
       <c r="D6" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E6" s="15">
         <v>44677.458333333336</v>
@@ -2508,7 +2508,7 @@
       </c>
       <c r="D7" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E7" s="15">
         <v>44678.458333333336</v>
@@ -2526,7 +2526,7 @@
       </c>
       <c r="D8" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E8" s="15">
         <v>44679.458333333336</v>
@@ -2544,7 +2544,7 @@
       </c>
       <c r="D9" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E9" s="15">
         <v>44680.458333333336</v>
@@ -2562,7 +2562,7 @@
       </c>
       <c r="D10" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E10" s="15">
         <v>44681.458333333336</v>
@@ -2580,7 +2580,7 @@
       </c>
       <c r="D11" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E11" s="15">
         <v>44682.458333333336</v>
@@ -2598,7 +2598,7 @@
       </c>
       <c r="D12" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E12" s="15">
         <v>44683.458333333336</v>
@@ -2616,7 +2616,7 @@
       </c>
       <c r="D13" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E13" s="15">
         <v>44684.458333333336</v>
@@ -2634,7 +2634,7 @@
       </c>
       <c r="D14" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E14" s="15">
         <v>44685.458333333336</v>
@@ -2652,7 +2652,7 @@
       </c>
       <c r="D15" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E15" s="15">
         <v>44686.458333333336</v>
@@ -2670,7 +2670,7 @@
       </c>
       <c r="D16" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E16" s="15">
         <v>44687.458333333336</v>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="D17" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E17" s="15">
         <v>44688.458333333336</v>
@@ -2706,7 +2706,7 @@
       </c>
       <c r="D18" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E18" s="15">
         <v>44689.458333333336</v>
@@ -2724,7 +2724,7 @@
       </c>
       <c r="D19" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E19" s="15">
         <v>44690.458333333336</v>
@@ -2742,7 +2742,7 @@
       </c>
       <c r="D20" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
       <c r="E20" s="15">
         <v>44691.458333333336</v>
@@ -2954,7 +2954,7 @@
       </c>
       <c r="F1" s="5">
         <f ca="1">NOW()</f>
-        <v>44411.600464236108</v>
+        <v>44412.768436458333</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3245,11 +3245,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C18"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="A1:B1"/>
@@ -3257,6 +3252,11 @@
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="B3:F3"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C18"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5965,8 +5965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C15CDDD0-1EC6-46EB-86DD-BB5C7073D9F7}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6950,8 +6950,8 @@
       <c r="H61" s="18"/>
       <c r="I61" s="68"/>
       <c r="J61" s="68"/>
-      <c r="L61" s="56">
-        <v>1</v>
+      <c r="L61" s="56" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.25">
@@ -6971,8 +6971,8 @@
       </c>
       <c r="H63" s="18"/>
       <c r="I63" s="67"/>
-      <c r="L63" s="61">
-        <v>1</v>
+      <c r="L63" s="61" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="64" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Docs: Se modifica normalización
</commit_message>
<xml_diff>
--- a/Primer_Trimestres/Nomalizacion/correccion/Normalización .xlsx
+++ b/Primer_Trimestres/Nomalizacion/correccion/Normalización .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Heelen\OneDrive\Documentos\GitHub\farmifarmacy1.0\Primer_Trimestres\Nomalizacion\correccion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d01d89a1400d5043/Documentos/GitHub/farmifarmacy1.0/Primer_Trimestres/Nomalizacion/correccion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AFA8DCF-3C1A-48DD-B7D9-62F7163A1C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{9AFA8DCF-3C1A-48DD-B7D9-62F7163A1C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF6A613F-2422-443E-89C2-D846455EAA86}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="3" activeTab="7" xr2:uid="{EB7CC955-6B47-4A67-9DA5-CC93A65E4CC7}"/>
   </bookViews>
@@ -27,12 +27,19 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="285">
   <si>
     <t>identificacion</t>
   </si>
@@ -1076,7 +1083,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1176,6 +1183,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1183,7 +1201,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1390,6 +1408,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -1496,61 +1526,6 @@
         <a:xfrm flipV="1">
           <a:off x="7200900" y="9334500"/>
           <a:ext cx="895350" cy="190501"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="tx2"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="Conector recto 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AC2B656-06AD-4029-AA09-C9503049EDCA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="10210800" y="8953500"/>
-          <a:ext cx="857250" cy="180976"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2671,7 +2646,7 @@
       </c>
       <c r="D2" s="15">
         <f ca="1">NOW()</f>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E2" s="15">
         <v>44673.458333333336</v>
@@ -2689,7 +2664,7 @@
       </c>
       <c r="D3" s="15">
         <f t="shared" ref="D3:D20" ca="1" si="0">NOW()</f>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E3" s="15">
         <v>44674.458333333336</v>
@@ -2707,7 +2682,7 @@
       </c>
       <c r="D4" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E4" s="15">
         <v>44675.458333333336</v>
@@ -2725,7 +2700,7 @@
       </c>
       <c r="D5" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E5" s="15">
         <v>44676.458333333336</v>
@@ -2743,7 +2718,7 @@
       </c>
       <c r="D6" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E6" s="15">
         <v>44677.458333333336</v>
@@ -2761,7 +2736,7 @@
       </c>
       <c r="D7" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E7" s="15">
         <v>44678.458333333336</v>
@@ -2779,7 +2754,7 @@
       </c>
       <c r="D8" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E8" s="15">
         <v>44679.458333333336</v>
@@ -2797,7 +2772,7 @@
       </c>
       <c r="D9" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E9" s="15">
         <v>44680.458333333336</v>
@@ -2815,7 +2790,7 @@
       </c>
       <c r="D10" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E10" s="15">
         <v>44681.458333333336</v>
@@ -2833,7 +2808,7 @@
       </c>
       <c r="D11" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E11" s="15">
         <v>44682.458333333336</v>
@@ -2851,7 +2826,7 @@
       </c>
       <c r="D12" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E12" s="15">
         <v>44683.458333333336</v>
@@ -2869,7 +2844,7 @@
       </c>
       <c r="D13" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E13" s="15">
         <v>44684.458333333336</v>
@@ -2887,7 +2862,7 @@
       </c>
       <c r="D14" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E14" s="15">
         <v>44685.458333333336</v>
@@ -2905,7 +2880,7 @@
       </c>
       <c r="D15" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E15" s="15">
         <v>44686.458333333336</v>
@@ -2923,7 +2898,7 @@
       </c>
       <c r="D16" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E16" s="15">
         <v>44687.458333333336</v>
@@ -2941,7 +2916,7 @@
       </c>
       <c r="D17" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E17" s="15">
         <v>44688.458333333336</v>
@@ -2959,7 +2934,7 @@
       </c>
       <c r="D18" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E18" s="15">
         <v>44689.458333333336</v>
@@ -2977,7 +2952,7 @@
       </c>
       <c r="D19" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E19" s="15">
         <v>44690.458333333336</v>
@@ -2995,7 +2970,7 @@
       </c>
       <c r="D20" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
       <c r="E20" s="15">
         <v>44691.458333333336</v>
@@ -3207,7 +3182,7 @@
       </c>
       <c r="F1" s="5">
         <f ca="1">NOW()</f>
-        <v>44426.910352083331</v>
+        <v>44480.914987847224</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3498,11 +3473,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C18"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="A1:B1"/>
@@ -3510,6 +3480,11 @@
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="B3:F3"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C18"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6327,8 +6302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C15CDDD0-1EC6-46EB-86DD-BB5C7073D9F7}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7087,7 +7062,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="29">
         <v>1014176160</v>
       </c>
@@ -7113,7 +7088,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="46">
         <v>1000350620</v>
       </c>
@@ -7137,7 +7112,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="38">
         <v>1016841206</v>
       </c>
@@ -7153,7 +7128,7 @@
       </c>
       <c r="K35" s="80"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="38">
         <v>1003275748</v>
       </c>
@@ -7161,7 +7136,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="38">
         <v>1011153857</v>
       </c>
@@ -7169,7 +7144,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="38">
         <v>1026238784</v>
       </c>
@@ -7177,7 +7152,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="38">
         <v>1011752470</v>
       </c>
@@ -7185,7 +7160,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="38">
         <v>1000016762</v>
       </c>
@@ -7193,7 +7168,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="38">
         <v>1021928374</v>
       </c>
@@ -7201,7 +7176,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="38">
         <v>1015159424</v>
       </c>
@@ -7209,7 +7184,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="38">
         <v>1009812763</v>
       </c>
@@ -7217,7 +7192,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="38">
         <v>10281927364</v>
       </c>
@@ -7225,18 +7200,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="80" t="s">
         <v>279</v>
       </c>
       <c r="B45" s="80"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L47" s="67">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I47" s="85">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L47" s="83"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B48" s="79" t="s">
         <v>283</v>
       </c>
@@ -7244,26 +7220,23 @@
       <c r="F48" s="66" t="s">
         <v>230</v>
       </c>
-      <c r="I48" s="67" t="s">
-        <v>230</v>
-      </c>
-      <c r="J48" s="67" t="s">
-        <v>230</v>
-      </c>
-      <c r="L48" s="79" t="s">
-        <v>255</v>
-      </c>
-      <c r="M48" s="79"/>
+      <c r="I48" s="85">
+        <v>1</v>
+      </c>
+      <c r="J48" s="83"/>
     </row>
     <row r="49" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C49" s="59">
         <v>1</v>
       </c>
-      <c r="F49" s="59">
+      <c r="F49" s="65">
         <v>1</v>
       </c>
-      <c r="I49" s="79" t="s">
-        <v>257</v>
+      <c r="G49" s="85" t="s">
+        <v>230</v>
+      </c>
+      <c r="I49" s="82" t="s">
+        <v>255</v>
       </c>
       <c r="J49" s="79"/>
     </row>
@@ -7274,7 +7247,7 @@
       <c r="F50" s="61" t="s">
         <v>230</v>
       </c>
-      <c r="G50" s="67">
+      <c r="G50" s="84">
         <v>1</v>
       </c>
     </row>
@@ -7434,7 +7407,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="18">
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="C53:D53"/>
     <mergeCell ref="C64:D64"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="G22:H22"/>
@@ -7450,10 +7426,6 @@
     <mergeCell ref="J35:K35"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="F51:G51"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="C53:D53"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>